<commit_message>
started updating burndown sheet:
</commit_message>
<xml_diff>
--- a/DesignDocs/Burndown.xlsx
+++ b/DesignDocs/Burndown.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\Jkenttechblog\DesignDocs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07B46BCC-933B-43FE-9BCA-15F58B4F917A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA1ACE92-E327-4C46-AE33-8EDEF79EBA5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="39">
   <si>
     <t>Product backlog ID</t>
   </si>
@@ -165,6 +165,30 @@
   </si>
   <si>
     <t>Completed Tasks</t>
+  </si>
+  <si>
+    <t>Create an Admin account</t>
+  </si>
+  <si>
+    <t>Login to AdminPortal</t>
+  </si>
+  <si>
+    <t>View admin dashboard</t>
+  </si>
+  <si>
+    <t>View logs</t>
+  </si>
+  <si>
+    <t>Create an article</t>
+  </si>
+  <si>
+    <t>View an article</t>
+  </si>
+  <si>
+    <t>View all articles</t>
+  </si>
+  <si>
+    <t>Search for article</t>
   </si>
 </sst>
 </file>
@@ -289,7 +313,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -339,9 +363,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3630,7 +3651,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3676,117 +3697,149 @@
       <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
+      <c r="B2" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="C2" s="15" t="str">
         <f t="shared" ref="C2:C12" si="0">IF(B2&lt;&gt;"","Jake","")</f>
-        <v/>
-      </c>
-      <c r="D2" s="7"/>
+        <v>Jake</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="E2" s="7"/>
       <c r="F2" s="7"/>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="str">
+      <c r="A3" s="6">
         <f t="shared" ref="A3:A14" si="1">IF(B3&lt;&gt;"",A2+1,"")</f>
-        <v/>
-      </c>
-      <c r="B3" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="C3" s="15" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D3" s="7"/>
+        <v>Jake</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="E3" s="7"/>
       <c r="F3" s="7"/>
       <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="str">
+      <c r="A4" s="6">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B4" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="C4" s="15" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D4" s="7"/>
+        <v>Jake</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>13</v>
+      </c>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="5"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="str">
+      <c r="A5" s="6">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B5" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="C5" s="15" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D5" s="7"/>
+        <v>Jake</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="5"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="str">
+      <c r="A6" s="6">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B6" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="C6" s="15" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D6" s="7"/>
+        <v>Jake</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="str">
+      <c r="A7" s="6">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B7" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="C7" s="15" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D7" s="7"/>
+        <v>Jake</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
       <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="str">
+      <c r="A8" s="6">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B8" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>37</v>
+      </c>
       <c r="C8" s="15" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D8" s="7"/>
+        <v>Jake</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>8</v>
+      </c>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
       <c r="G8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="str">
+      <c r="A9" s="6">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B9" s="5"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="C9" s="15" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="D9" s="7"/>
+        <v>Jake</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
       <c r="G9" s="5"/>
@@ -7455,44 +7508,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24" t="s">
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="22" t="s">
         <v>14</v>
       </c>
@@ -7514,7 +7567,7 @@
       <c r="M2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="24"/>
+      <c r="N2" s="23"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
@@ -13302,11 +13355,11 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="16">
-        <f>DATE(YEAR(A2), MONTH(A2),DAY( A2+1))</f>
+        <f t="shared" ref="A3:A8" si="0">DATE(YEAR(A2), MONTH(A2),DAY( A2+1))</f>
         <v>45306</v>
       </c>
       <c r="B3" s="17">
-        <f t="shared" ref="B3:B8" si="0">B2-($B$2/6)</f>
+        <f t="shared" ref="B3:B8" si="1">B2-($B$2/6)</f>
         <v>0</v>
       </c>
       <c r="C3" s="1">
@@ -13320,15 +13373,15 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="16">
-        <f>DATE(YEAR(A3), MONTH(A3),DAY( A3+1))</f>
+        <f t="shared" si="0"/>
         <v>45307</v>
       </c>
       <c r="B4" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4:C8" si="1">C3-D3</f>
+        <f t="shared" ref="C4:C8" si="2">C3-D3</f>
         <v>0</v>
       </c>
       <c r="D4" s="1">
@@ -13338,15 +13391,15 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="16">
-        <f>DATE(YEAR(A4), MONTH(A4),DAY( A4+1))</f>
+        <f t="shared" si="0"/>
         <v>45308</v>
       </c>
       <c r="B5" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D5" s="1">
@@ -13356,15 +13409,15 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="16">
-        <f>DATE(YEAR(A5), MONTH(A5),DAY( A5+1))</f>
+        <f t="shared" si="0"/>
         <v>45309</v>
       </c>
       <c r="B6" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D6" s="1">
@@ -13374,15 +13427,15 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="16">
-        <f>DATE(YEAR(A6), MONTH(A6),DAY( A6+1))</f>
+        <f t="shared" si="0"/>
         <v>45310</v>
       </c>
       <c r="B7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D7" s="1">
@@ -13392,15 +13445,15 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="16">
-        <f>DATE(YEAR(A7), MONTH(A7),DAY( A7+1))</f>
+        <f t="shared" si="0"/>
         <v>45311</v>
       </c>
       <c r="B8" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D8" s="1">
@@ -13453,66 +13506,66 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="24" t="s">
+      <c r="E1" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="24" t="s">
+      <c r="F1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
-      <c r="M1" s="24"/>
-      <c r="N1" s="24" t="s">
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26"/>
-      <c r="B2" s="24"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="23" t="s">
+      <c r="A2" s="25"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="23" t="s">
+      <c r="H2" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="23" t="s">
+      <c r="I2" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="23" t="s">
+      <c r="K2" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="23" t="s">
+      <c r="L2" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="23" t="s">
+      <c r="M2" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="N2" s="24"/>
+      <c r="N2" s="23"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
@@ -14080,7 +14133,7 @@
         <v/>
       </c>
       <c r="C23" s="6" t="str">
-        <f t="shared" ref="C3:C66" si="1">IF(ISBLANK(A23),"",IF(A23&lt;&gt;A22,A23+0.1,C22+0.1))</f>
+        <f t="shared" ref="C23:C66" si="1">IF(ISBLANK(A23),"",IF(A23&lt;&gt;A22,A23+0.1,C22+0.1))</f>
         <v/>
       </c>
       <c r="D23" s="5"/>
@@ -19300,11 +19353,11 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="16">
-        <f>DATE(YEAR(A2), MONTH(A2),DAY( A2+1))</f>
+        <f t="shared" ref="A3:A8" si="0">DATE(YEAR(A2), MONTH(A2),DAY( A2+1))</f>
         <v>45306</v>
       </c>
       <c r="B3" s="17">
-        <f t="shared" ref="B3:B8" si="0">B2-($B$2/6)</f>
+        <f t="shared" ref="B3:B8" si="1">B2-($B$2/6)</f>
         <v>0</v>
       </c>
       <c r="C3" s="1">
@@ -19318,15 +19371,15 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="16">
-        <f>DATE(YEAR(A3), MONTH(A3),DAY( A3+1))</f>
+        <f t="shared" si="0"/>
         <v>45307</v>
       </c>
       <c r="B4" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C4" s="1">
-        <f t="shared" ref="C4:C8" si="1">C3-D3</f>
+        <f t="shared" ref="C4:C8" si="2">C3-D3</f>
         <v>0</v>
       </c>
       <c r="D4" s="1">
@@ -19336,15 +19389,15 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="16">
-        <f>DATE(YEAR(A4), MONTH(A4),DAY( A4+1))</f>
+        <f t="shared" si="0"/>
         <v>45308</v>
       </c>
       <c r="B5" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D5" s="1">
@@ -19354,15 +19407,15 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="16">
-        <f>DATE(YEAR(A5), MONTH(A5),DAY( A5+1))</f>
+        <f t="shared" si="0"/>
         <v>45309</v>
       </c>
       <c r="B6" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D6" s="1">
@@ -19372,15 +19425,15 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="16">
-        <f>DATE(YEAR(A6), MONTH(A6),DAY( A6+1))</f>
+        <f t="shared" si="0"/>
         <v>45310</v>
       </c>
       <c r="B7" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D7" s="1">
@@ -19390,15 +19443,15 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="16">
-        <f>DATE(YEAR(A7), MONTH(A7),DAY( A7+1))</f>
+        <f t="shared" si="0"/>
         <v>45311</v>
       </c>
       <c r="B8" s="17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="C8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="D8" s="1">
@@ -19963,14 +20016,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="d12b44e9-a355-4801-8c10-af0fa875eb52" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5517439e-c63d-4269-a460-349c4f0e575b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20157,21 +20208,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d12b44e9-a355-4801-8c10-af0fa875eb52" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="5517439e-c63d-4269-a460-349c4f0e575b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A769E7B-2011-4CCB-A1CB-4C5F3F198FFB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{531A822F-48A0-46FD-9A7C-C24C615E1364}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d12b44e9-a355-4801-8c10-af0fa875eb52"/>
-    <ds:schemaRef ds:uri="5517439e-c63d-4269-a460-349c4f0e575b"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20196,9 +20246,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{531A822F-48A0-46FD-9A7C-C24C615E1364}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A769E7B-2011-4CCB-A1CB-4C5F3F198FFB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d12b44e9-a355-4801-8c10-af0fa875eb52"/>
+    <ds:schemaRef ds:uri="5517439e-c63d-4269-a460-349c4f0e575b"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>